<commit_message>
modify: update for confidence interval of corr
</commit_message>
<xml_diff>
--- a/WPCN/2020_11_additional_test/overall_report.xlsx
+++ b/WPCN/2020_11_additional_test/overall_report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -151,6 +151,10 @@
   </si>
   <si>
     <t>3. create more test data to increase accuracy of test result?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. using XAI to find the reason for (size=12, WDs=6, No.=3)?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -535,33 +539,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -586,12 +563,6 @@
     <xf numFmtId="179" fontId="9" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="11" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -607,12 +578,6 @@
     <xf numFmtId="179" fontId="14" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="10" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -627,6 +592,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1150,10 +1154,10 @@
   <dimension ref="A1:Q630"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C608" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N618" sqref="N618"/>
+      <selection pane="bottomRight" activeCell="M124" sqref="M124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1661,13 +1665,13 @@
         <f t="shared" si="1"/>
         <v>0.354875</v>
       </c>
-      <c r="M10" s="21" t="s">
+      <c r="M10" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="23"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="50"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="9">
@@ -1705,11 +1709,11 @@
         <f t="shared" si="1"/>
         <v>0.28862500000000002</v>
       </c>
-      <c r="M11" s="24"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="26"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="41"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="9">
@@ -1747,11 +1751,11 @@
         <f t="shared" si="1"/>
         <v>0.39724999999999999</v>
       </c>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="26"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="41"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="9">
@@ -1789,11 +1793,11 @@
         <f t="shared" si="1"/>
         <v>0.46300000000000002</v>
       </c>
-      <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="41"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="9">
@@ -1831,11 +1835,11 @@
         <f t="shared" si="1"/>
         <v>0.31662499999999999</v>
       </c>
-      <c r="M14" s="24"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="26"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="41"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="9">
@@ -1873,11 +1877,11 @@
         <f t="shared" si="1"/>
         <v>0.48399999999999999</v>
       </c>
-      <c r="M15" s="24"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="26"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="41"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="9">
@@ -1915,11 +1919,11 @@
         <f t="shared" si="1"/>
         <v>0.34937499999999999</v>
       </c>
-      <c r="M16" s="24"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="26"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="41"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" s="9">
@@ -1957,11 +1961,11 @@
         <f t="shared" si="1"/>
         <v>0.33487499999999998</v>
       </c>
-      <c r="M17" s="24"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="26"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="41"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" s="9">
@@ -1999,11 +2003,11 @@
         <f t="shared" si="1"/>
         <v>0.391125</v>
       </c>
-      <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="26"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="41"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" s="9">
@@ -2041,11 +2045,11 @@
         <f t="shared" si="1"/>
         <v>0.60112500000000002</v>
       </c>
-      <c r="M19" s="24"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="26"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="41"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" s="9">
@@ -2083,11 +2087,11 @@
         <f t="shared" si="1"/>
         <v>0.35025000000000001</v>
       </c>
-      <c r="M20" s="24"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="26"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="41"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" s="9">
@@ -2125,11 +2129,11 @@
         <f t="shared" si="1"/>
         <v>0.48675000000000002</v>
       </c>
-      <c r="M21" s="24"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="26"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="41"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" s="9">
@@ -2167,11 +2171,11 @@
         <f t="shared" si="1"/>
         <v>0.57487500000000002</v>
       </c>
-      <c r="M22" s="24"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="26"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="41"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" s="9">
@@ -2209,11 +2213,11 @@
         <f t="shared" si="1"/>
         <v>0.420375</v>
       </c>
-      <c r="M23" s="24"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="26"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="41"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" s="9">
@@ -2251,11 +2255,11 @@
         <f t="shared" si="1"/>
         <v>0.58862499999999995</v>
       </c>
-      <c r="M24" s="24"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="26"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="41"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" s="9">
@@ -2293,11 +2297,11 @@
         <f t="shared" si="1"/>
         <v>0.43525000000000003</v>
       </c>
-      <c r="M25" s="24"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="26"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="41"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" s="9">
@@ -2335,11 +2339,11 @@
         <f t="shared" si="1"/>
         <v>0.54774999999999996</v>
       </c>
-      <c r="M26" s="27"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="29"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="44"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" s="9">
@@ -2414,13 +2418,13 @@
         <f t="shared" si="1"/>
         <v>0.43325000000000002</v>
       </c>
-      <c r="M28" s="21" t="s">
+      <c r="M28" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="23"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="50"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" s="9">
@@ -2458,11 +2462,11 @@
         <f t="shared" si="1"/>
         <v>0.33975</v>
       </c>
-      <c r="M29" s="24"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="26"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="41"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" s="9">
@@ -2500,11 +2504,11 @@
         <f t="shared" si="1"/>
         <v>0.453625</v>
       </c>
-      <c r="M30" s="24"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
-      <c r="Q30" s="26"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="41"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" s="9">
@@ -2542,11 +2546,11 @@
         <f t="shared" si="1"/>
         <v>0.33975</v>
       </c>
-      <c r="M31" s="24"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
-      <c r="Q31" s="26"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="41"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" s="9">
@@ -2584,11 +2588,11 @@
         <f t="shared" si="1"/>
         <v>0.42925000000000002</v>
       </c>
-      <c r="M32" s="24"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
-      <c r="P32" s="25"/>
-      <c r="Q32" s="26"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="40"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="40"/>
+      <c r="Q32" s="41"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33" s="9">
@@ -2626,11 +2630,11 @@
         <f t="shared" si="1"/>
         <v>0.47275</v>
       </c>
-      <c r="M33" s="24"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="26"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="41"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A34" s="9">
@@ -2668,11 +2672,11 @@
         <f t="shared" si="1"/>
         <v>0.45137500000000003</v>
       </c>
-      <c r="M34" s="24"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="25"/>
-      <c r="Q34" s="26"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="41"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A35" s="9">
@@ -2710,11 +2714,11 @@
         <f t="shared" si="1"/>
         <v>0.45850000000000002</v>
       </c>
-      <c r="M35" s="24"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="26"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="40"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="40"/>
+      <c r="Q35" s="41"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A36" s="9">
@@ -2752,11 +2756,11 @@
         <f t="shared" si="1"/>
         <v>0.43012499999999998</v>
       </c>
-      <c r="M36" s="24"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="26"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="40"/>
+      <c r="Q36" s="41"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A37" s="9">
@@ -2794,11 +2798,11 @@
         <f t="shared" si="1"/>
         <v>0.46012500000000001</v>
       </c>
-      <c r="M37" s="24"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="25"/>
-      <c r="P37" s="25"/>
-      <c r="Q37" s="26"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="40"/>
+      <c r="O37" s="40"/>
+      <c r="P37" s="40"/>
+      <c r="Q37" s="41"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A38" s="9">
@@ -2836,11 +2840,11 @@
         <f t="shared" si="1"/>
         <v>0.56687500000000002</v>
       </c>
-      <c r="M38" s="24"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="25"/>
-      <c r="P38" s="25"/>
-      <c r="Q38" s="26"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="40"/>
+      <c r="O38" s="40"/>
+      <c r="P38" s="40"/>
+      <c r="Q38" s="41"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A39" s="9">
@@ -2878,11 +2882,11 @@
         <f t="shared" si="1"/>
         <v>0.41112500000000002</v>
       </c>
-      <c r="M39" s="24"/>
-      <c r="N39" s="25"/>
-      <c r="O39" s="25"/>
-      <c r="P39" s="25"/>
-      <c r="Q39" s="26"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="40"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="40"/>
+      <c r="Q39" s="41"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A40" s="9">
@@ -2920,11 +2924,11 @@
         <f t="shared" si="1"/>
         <v>0.5645</v>
       </c>
-      <c r="M40" s="24"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="25"/>
-      <c r="P40" s="25"/>
-      <c r="Q40" s="26"/>
+      <c r="M40" s="39"/>
+      <c r="N40" s="40"/>
+      <c r="O40" s="40"/>
+      <c r="P40" s="40"/>
+      <c r="Q40" s="41"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A41" s="9">
@@ -2962,11 +2966,11 @@
         <f t="shared" si="1"/>
         <v>0.40112500000000001</v>
       </c>
-      <c r="M41" s="24"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="25"/>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="26"/>
+      <c r="M41" s="39"/>
+      <c r="N41" s="40"/>
+      <c r="O41" s="40"/>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="41"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A42" s="9">
@@ -3004,11 +3008,11 @@
         <f t="shared" si="1"/>
         <v>0.55562500000000004</v>
       </c>
-      <c r="M42" s="24"/>
-      <c r="N42" s="25"/>
-      <c r="O42" s="25"/>
-      <c r="P42" s="25"/>
-      <c r="Q42" s="26"/>
+      <c r="M42" s="39"/>
+      <c r="N42" s="40"/>
+      <c r="O42" s="40"/>
+      <c r="P42" s="40"/>
+      <c r="Q42" s="41"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A43" s="9">
@@ -3046,11 +3050,11 @@
         <f t="shared" si="1"/>
         <v>0.45100000000000001</v>
       </c>
-      <c r="M43" s="24"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="25"/>
-      <c r="P43" s="25"/>
-      <c r="Q43" s="26"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="40"/>
+      <c r="O43" s="40"/>
+      <c r="P43" s="40"/>
+      <c r="Q43" s="41"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A44" s="9">
@@ -3088,11 +3092,11 @@
         <f t="shared" si="1"/>
         <v>0.39787499999999998</v>
       </c>
-      <c r="M44" s="27"/>
-      <c r="N44" s="28"/>
-      <c r="O44" s="28"/>
-      <c r="P44" s="28"/>
-      <c r="Q44" s="29"/>
+      <c r="M44" s="42"/>
+      <c r="N44" s="43"/>
+      <c r="O44" s="43"/>
+      <c r="P44" s="43"/>
+      <c r="Q44" s="44"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A45" s="9">
@@ -3167,13 +3171,13 @@
         <f t="shared" si="1"/>
         <v>0.31362499999999999</v>
       </c>
-      <c r="M46" s="21" t="s">
+      <c r="M46" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="23"/>
+      <c r="N46" s="49"/>
+      <c r="O46" s="49"/>
+      <c r="P46" s="49"/>
+      <c r="Q46" s="50"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A47" s="9">
@@ -3211,11 +3215,11 @@
         <f t="shared" si="1"/>
         <v>0.55812499999999998</v>
       </c>
-      <c r="M47" s="24"/>
-      <c r="N47" s="25"/>
-      <c r="O47" s="25"/>
-      <c r="P47" s="25"/>
-      <c r="Q47" s="26"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="40"/>
+      <c r="O47" s="40"/>
+      <c r="P47" s="40"/>
+      <c r="Q47" s="41"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A48" s="9">
@@ -3253,11 +3257,11 @@
         <f t="shared" si="1"/>
         <v>0.32174999999999998</v>
       </c>
-      <c r="M48" s="24"/>
-      <c r="N48" s="25"/>
-      <c r="O48" s="25"/>
-      <c r="P48" s="25"/>
-      <c r="Q48" s="26"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="40"/>
+      <c r="O48" s="40"/>
+      <c r="P48" s="40"/>
+      <c r="Q48" s="41"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A49" s="9">
@@ -3295,11 +3299,11 @@
         <f t="shared" si="1"/>
         <v>0.53112499999999996</v>
       </c>
-      <c r="M49" s="24"/>
-      <c r="N49" s="25"/>
-      <c r="O49" s="25"/>
-      <c r="P49" s="25"/>
-      <c r="Q49" s="26"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="40"/>
+      <c r="O49" s="40"/>
+      <c r="P49" s="40"/>
+      <c r="Q49" s="41"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A50" s="9">
@@ -3337,11 +3341,11 @@
         <f t="shared" si="1"/>
         <v>0.41849999999999998</v>
       </c>
-      <c r="M50" s="24"/>
-      <c r="N50" s="25"/>
-      <c r="O50" s="25"/>
-      <c r="P50" s="25"/>
-      <c r="Q50" s="26"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="40"/>
+      <c r="O50" s="40"/>
+      <c r="P50" s="40"/>
+      <c r="Q50" s="41"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A51" s="9">
@@ -3379,11 +3383,11 @@
         <f t="shared" si="1"/>
         <v>0.38987500000000003</v>
       </c>
-      <c r="M51" s="24"/>
-      <c r="N51" s="25"/>
-      <c r="O51" s="25"/>
-      <c r="P51" s="25"/>
-      <c r="Q51" s="26"/>
+      <c r="M51" s="39"/>
+      <c r="N51" s="40"/>
+      <c r="O51" s="40"/>
+      <c r="P51" s="40"/>
+      <c r="Q51" s="41"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A52" s="9">
@@ -3421,11 +3425,11 @@
         <f t="shared" si="1"/>
         <v>0.50562499999999999</v>
       </c>
-      <c r="M52" s="24"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="25"/>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="26"/>
+      <c r="M52" s="39"/>
+      <c r="N52" s="40"/>
+      <c r="O52" s="40"/>
+      <c r="P52" s="40"/>
+      <c r="Q52" s="41"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A53" s="9">
@@ -3463,11 +3467,11 @@
         <f t="shared" si="1"/>
         <v>0.43099999999999999</v>
       </c>
-      <c r="M53" s="24"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="25"/>
-      <c r="P53" s="25"/>
-      <c r="Q53" s="26"/>
+      <c r="M53" s="39"/>
+      <c r="N53" s="40"/>
+      <c r="O53" s="40"/>
+      <c r="P53" s="40"/>
+      <c r="Q53" s="41"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A54" s="9">
@@ -3505,11 +3509,11 @@
         <f t="shared" si="1"/>
         <v>0.35775000000000001</v>
       </c>
-      <c r="M54" s="24"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="25"/>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="26"/>
+      <c r="M54" s="39"/>
+      <c r="N54" s="40"/>
+      <c r="O54" s="40"/>
+      <c r="P54" s="40"/>
+      <c r="Q54" s="41"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A55" s="9">
@@ -3547,11 +3551,11 @@
         <f t="shared" si="1"/>
         <v>0.56174999999999997</v>
       </c>
-      <c r="M55" s="24"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="26"/>
+      <c r="M55" s="39"/>
+      <c r="N55" s="40"/>
+      <c r="O55" s="40"/>
+      <c r="P55" s="40"/>
+      <c r="Q55" s="41"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A56" s="9">
@@ -3589,11 +3593,11 @@
         <f t="shared" si="1"/>
         <v>0.41025</v>
       </c>
-      <c r="M56" s="24"/>
-      <c r="N56" s="25"/>
-      <c r="O56" s="25"/>
-      <c r="P56" s="25"/>
-      <c r="Q56" s="26"/>
+      <c r="M56" s="39"/>
+      <c r="N56" s="40"/>
+      <c r="O56" s="40"/>
+      <c r="P56" s="40"/>
+      <c r="Q56" s="41"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A57" s="9">
@@ -3631,11 +3635,11 @@
         <f t="shared" si="1"/>
         <v>0.48249999999999998</v>
       </c>
-      <c r="M57" s="24"/>
-      <c r="N57" s="25"/>
-      <c r="O57" s="25"/>
-      <c r="P57" s="25"/>
-      <c r="Q57" s="26"/>
+      <c r="M57" s="39"/>
+      <c r="N57" s="40"/>
+      <c r="O57" s="40"/>
+      <c r="P57" s="40"/>
+      <c r="Q57" s="41"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A58" s="9">
@@ -3673,11 +3677,11 @@
         <f t="shared" si="1"/>
         <v>0.423375</v>
       </c>
-      <c r="M58" s="24"/>
-      <c r="N58" s="25"/>
-      <c r="O58" s="25"/>
-      <c r="P58" s="25"/>
-      <c r="Q58" s="26"/>
+      <c r="M58" s="39"/>
+      <c r="N58" s="40"/>
+      <c r="O58" s="40"/>
+      <c r="P58" s="40"/>
+      <c r="Q58" s="41"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A59" s="9">
@@ -3715,11 +3719,11 @@
         <f t="shared" si="1"/>
         <v>0.51300000000000001</v>
       </c>
-      <c r="M59" s="24"/>
-      <c r="N59" s="25"/>
-      <c r="O59" s="25"/>
-      <c r="P59" s="25"/>
-      <c r="Q59" s="26"/>
+      <c r="M59" s="39"/>
+      <c r="N59" s="40"/>
+      <c r="O59" s="40"/>
+      <c r="P59" s="40"/>
+      <c r="Q59" s="41"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A60" s="9">
@@ -3757,11 +3761,11 @@
         <f t="shared" si="1"/>
         <v>0.56762500000000005</v>
       </c>
-      <c r="M60" s="24"/>
-      <c r="N60" s="25"/>
-      <c r="O60" s="25"/>
-      <c r="P60" s="25"/>
-      <c r="Q60" s="26"/>
+      <c r="M60" s="39"/>
+      <c r="N60" s="40"/>
+      <c r="O60" s="40"/>
+      <c r="P60" s="40"/>
+      <c r="Q60" s="41"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A61" s="9">
@@ -3799,11 +3803,11 @@
         <f t="shared" si="1"/>
         <v>0.30287500000000001</v>
       </c>
-      <c r="M61" s="24"/>
-      <c r="N61" s="25"/>
-      <c r="O61" s="25"/>
-      <c r="P61" s="25"/>
-      <c r="Q61" s="26"/>
+      <c r="M61" s="39"/>
+      <c r="N61" s="40"/>
+      <c r="O61" s="40"/>
+      <c r="P61" s="40"/>
+      <c r="Q61" s="41"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A62" s="9">
@@ -3841,11 +3845,11 @@
         <f t="shared" si="1"/>
         <v>0.43087500000000001</v>
       </c>
-      <c r="M62" s="27"/>
-      <c r="N62" s="28"/>
-      <c r="O62" s="28"/>
-      <c r="P62" s="28"/>
-      <c r="Q62" s="29"/>
+      <c r="M62" s="42"/>
+      <c r="N62" s="43"/>
+      <c r="O62" s="43"/>
+      <c r="P62" s="43"/>
+      <c r="Q62" s="44"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A63" s="9">
@@ -3920,13 +3924,13 @@
         <f t="shared" si="1"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="M64" s="21" t="s">
+      <c r="M64" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="N64" s="22"/>
-      <c r="O64" s="22"/>
-      <c r="P64" s="22"/>
-      <c r="Q64" s="23"/>
+      <c r="N64" s="49"/>
+      <c r="O64" s="49"/>
+      <c r="P64" s="49"/>
+      <c r="Q64" s="50"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A65" s="9">
@@ -3964,11 +3968,11 @@
         <f t="shared" si="1"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="M65" s="24"/>
-      <c r="N65" s="25"/>
-      <c r="O65" s="25"/>
-      <c r="P65" s="25"/>
-      <c r="Q65" s="26"/>
+      <c r="M65" s="39"/>
+      <c r="N65" s="40"/>
+      <c r="O65" s="40"/>
+      <c r="P65" s="40"/>
+      <c r="Q65" s="41"/>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A66" s="9">
@@ -4006,11 +4010,11 @@
         <f t="shared" si="1"/>
         <v>0.640625</v>
       </c>
-      <c r="M66" s="24"/>
-      <c r="N66" s="25"/>
-      <c r="O66" s="25"/>
-      <c r="P66" s="25"/>
-      <c r="Q66" s="26"/>
+      <c r="M66" s="39"/>
+      <c r="N66" s="40"/>
+      <c r="O66" s="40"/>
+      <c r="P66" s="40"/>
+      <c r="Q66" s="41"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A67" s="9">
@@ -4048,11 +4052,11 @@
         <f t="shared" ref="K67:K130" si="6">E67/A67</f>
         <v>0.28912500000000002</v>
       </c>
-      <c r="M67" s="24"/>
-      <c r="N67" s="25"/>
-      <c r="O67" s="25"/>
-      <c r="P67" s="25"/>
-      <c r="Q67" s="26"/>
+      <c r="M67" s="39"/>
+      <c r="N67" s="40"/>
+      <c r="O67" s="40"/>
+      <c r="P67" s="40"/>
+      <c r="Q67" s="41"/>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A68" s="9">
@@ -4090,11 +4094,11 @@
         <f t="shared" si="6"/>
         <v>0.52249999999999996</v>
       </c>
-      <c r="M68" s="24"/>
-      <c r="N68" s="25"/>
-      <c r="O68" s="25"/>
-      <c r="P68" s="25"/>
-      <c r="Q68" s="26"/>
+      <c r="M68" s="39"/>
+      <c r="N68" s="40"/>
+      <c r="O68" s="40"/>
+      <c r="P68" s="40"/>
+      <c r="Q68" s="41"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A69" s="9">
@@ -4132,11 +4136,11 @@
         <f t="shared" si="6"/>
         <v>0.33137499999999998</v>
       </c>
-      <c r="M69" s="24"/>
-      <c r="N69" s="25"/>
-      <c r="O69" s="25"/>
-      <c r="P69" s="25"/>
-      <c r="Q69" s="26"/>
+      <c r="M69" s="39"/>
+      <c r="N69" s="40"/>
+      <c r="O69" s="40"/>
+      <c r="P69" s="40"/>
+      <c r="Q69" s="41"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A70" s="9">
@@ -4174,11 +4178,11 @@
         <f t="shared" si="6"/>
         <v>0.41387499999999999</v>
       </c>
-      <c r="M70" s="24"/>
-      <c r="N70" s="25"/>
-      <c r="O70" s="25"/>
-      <c r="P70" s="25"/>
-      <c r="Q70" s="26"/>
+      <c r="M70" s="39"/>
+      <c r="N70" s="40"/>
+      <c r="O70" s="40"/>
+      <c r="P70" s="40"/>
+      <c r="Q70" s="41"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A71" s="9">
@@ -4216,11 +4220,11 @@
         <f t="shared" si="6"/>
         <v>0.41325000000000001</v>
       </c>
-      <c r="M71" s="24"/>
-      <c r="N71" s="25"/>
-      <c r="O71" s="25"/>
-      <c r="P71" s="25"/>
-      <c r="Q71" s="26"/>
+      <c r="M71" s="39"/>
+      <c r="N71" s="40"/>
+      <c r="O71" s="40"/>
+      <c r="P71" s="40"/>
+      <c r="Q71" s="41"/>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A72" s="9">
@@ -4258,11 +4262,11 @@
         <f t="shared" si="6"/>
         <v>0.42412499999999997</v>
       </c>
-      <c r="M72" s="24"/>
-      <c r="N72" s="25"/>
-      <c r="O72" s="25"/>
-      <c r="P72" s="25"/>
-      <c r="Q72" s="26"/>
+      <c r="M72" s="39"/>
+      <c r="N72" s="40"/>
+      <c r="O72" s="40"/>
+      <c r="P72" s="40"/>
+      <c r="Q72" s="41"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A73" s="9">
@@ -4300,11 +4304,11 @@
         <f t="shared" si="6"/>
         <v>0.56062500000000004</v>
       </c>
-      <c r="M73" s="24"/>
-      <c r="N73" s="25"/>
-      <c r="O73" s="25"/>
-      <c r="P73" s="25"/>
-      <c r="Q73" s="26"/>
+      <c r="M73" s="39"/>
+      <c r="N73" s="40"/>
+      <c r="O73" s="40"/>
+      <c r="P73" s="40"/>
+      <c r="Q73" s="41"/>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A74" s="9">
@@ -4342,11 +4346,11 @@
         <f t="shared" si="6"/>
         <v>0.40300000000000002</v>
       </c>
-      <c r="M74" s="24"/>
-      <c r="N74" s="25"/>
-      <c r="O74" s="25"/>
-      <c r="P74" s="25"/>
-      <c r="Q74" s="26"/>
+      <c r="M74" s="39"/>
+      <c r="N74" s="40"/>
+      <c r="O74" s="40"/>
+      <c r="P74" s="40"/>
+      <c r="Q74" s="41"/>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A75" s="9">
@@ -4384,11 +4388,11 @@
         <f t="shared" si="6"/>
         <v>0.42099999999999999</v>
       </c>
-      <c r="M75" s="24"/>
-      <c r="N75" s="25"/>
-      <c r="O75" s="25"/>
-      <c r="P75" s="25"/>
-      <c r="Q75" s="26"/>
+      <c r="M75" s="39"/>
+      <c r="N75" s="40"/>
+      <c r="O75" s="40"/>
+      <c r="P75" s="40"/>
+      <c r="Q75" s="41"/>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A76" s="9">
@@ -4426,11 +4430,11 @@
         <f t="shared" si="6"/>
         <v>0.32162499999999999</v>
       </c>
-      <c r="M76" s="24"/>
-      <c r="N76" s="25"/>
-      <c r="O76" s="25"/>
-      <c r="P76" s="25"/>
-      <c r="Q76" s="26"/>
+      <c r="M76" s="39"/>
+      <c r="N76" s="40"/>
+      <c r="O76" s="40"/>
+      <c r="P76" s="40"/>
+      <c r="Q76" s="41"/>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A77" s="9">
@@ -4468,11 +4472,11 @@
         <f t="shared" si="6"/>
         <v>0.55312499999999998</v>
       </c>
-      <c r="M77" s="24"/>
-      <c r="N77" s="25"/>
-      <c r="O77" s="25"/>
-      <c r="P77" s="25"/>
-      <c r="Q77" s="26"/>
+      <c r="M77" s="39"/>
+      <c r="N77" s="40"/>
+      <c r="O77" s="40"/>
+      <c r="P77" s="40"/>
+      <c r="Q77" s="41"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A78" s="9">
@@ -4510,11 +4514,11 @@
         <f t="shared" si="6"/>
         <v>0.59775</v>
       </c>
-      <c r="M78" s="24"/>
-      <c r="N78" s="25"/>
-      <c r="O78" s="25"/>
-      <c r="P78" s="25"/>
-      <c r="Q78" s="26"/>
+      <c r="M78" s="39"/>
+      <c r="N78" s="40"/>
+      <c r="O78" s="40"/>
+      <c r="P78" s="40"/>
+      <c r="Q78" s="41"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A79" s="9">
@@ -4552,11 +4556,11 @@
         <f t="shared" si="6"/>
         <v>0.42375000000000002</v>
       </c>
-      <c r="M79" s="24"/>
-      <c r="N79" s="25"/>
-      <c r="O79" s="25"/>
-      <c r="P79" s="25"/>
-      <c r="Q79" s="26"/>
+      <c r="M79" s="39"/>
+      <c r="N79" s="40"/>
+      <c r="O79" s="40"/>
+      <c r="P79" s="40"/>
+      <c r="Q79" s="41"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A80" s="9">
@@ -4594,11 +4598,11 @@
         <f t="shared" si="6"/>
         <v>0.43812499999999999</v>
       </c>
-      <c r="M80" s="27"/>
-      <c r="N80" s="28"/>
-      <c r="O80" s="28"/>
-      <c r="P80" s="28"/>
-      <c r="Q80" s="29"/>
+      <c r="M80" s="42"/>
+      <c r="N80" s="43"/>
+      <c r="O80" s="43"/>
+      <c r="P80" s="43"/>
+      <c r="Q80" s="44"/>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A81" s="9">
@@ -4673,13 +4677,13 @@
         <f t="shared" si="6"/>
         <v>0.50362499999999999</v>
       </c>
-      <c r="M82" s="21" t="s">
+      <c r="M82" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="N82" s="22"/>
-      <c r="O82" s="22"/>
-      <c r="P82" s="22"/>
-      <c r="Q82" s="23"/>
+      <c r="N82" s="49"/>
+      <c r="O82" s="49"/>
+      <c r="P82" s="49"/>
+      <c r="Q82" s="50"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A83" s="9">
@@ -4717,11 +4721,11 @@
         <f t="shared" si="6"/>
         <v>0.38162499999999999</v>
       </c>
-      <c r="M83" s="24"/>
-      <c r="N83" s="25"/>
-      <c r="O83" s="25"/>
-      <c r="P83" s="25"/>
-      <c r="Q83" s="26"/>
+      <c r="M83" s="39"/>
+      <c r="N83" s="40"/>
+      <c r="O83" s="40"/>
+      <c r="P83" s="40"/>
+      <c r="Q83" s="41"/>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A84" s="9">
@@ -4759,11 +4763,11 @@
         <f t="shared" si="6"/>
         <v>0.44350000000000001</v>
       </c>
-      <c r="M84" s="24"/>
-      <c r="N84" s="25"/>
-      <c r="O84" s="25"/>
-      <c r="P84" s="25"/>
-      <c r="Q84" s="26"/>
+      <c r="M84" s="39"/>
+      <c r="N84" s="40"/>
+      <c r="O84" s="40"/>
+      <c r="P84" s="40"/>
+      <c r="Q84" s="41"/>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A85" s="9">
@@ -4801,11 +4805,11 @@
         <f t="shared" si="6"/>
         <v>0.46187499999999998</v>
       </c>
-      <c r="M85" s="24"/>
-      <c r="N85" s="25"/>
-      <c r="O85" s="25"/>
-      <c r="P85" s="25"/>
-      <c r="Q85" s="26"/>
+      <c r="M85" s="39"/>
+      <c r="N85" s="40"/>
+      <c r="O85" s="40"/>
+      <c r="P85" s="40"/>
+      <c r="Q85" s="41"/>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A86" s="9">
@@ -4843,11 +4847,11 @@
         <f t="shared" si="6"/>
         <v>0.47137499999999999</v>
       </c>
-      <c r="M86" s="24"/>
-      <c r="N86" s="25"/>
-      <c r="O86" s="25"/>
-      <c r="P86" s="25"/>
-      <c r="Q86" s="26"/>
+      <c r="M86" s="39"/>
+      <c r="N86" s="40"/>
+      <c r="O86" s="40"/>
+      <c r="P86" s="40"/>
+      <c r="Q86" s="41"/>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A87" s="9">
@@ -4885,11 +4889,11 @@
         <f t="shared" si="6"/>
         <v>0.35375000000000001</v>
       </c>
-      <c r="M87" s="24"/>
-      <c r="N87" s="25"/>
-      <c r="O87" s="25"/>
-      <c r="P87" s="25"/>
-      <c r="Q87" s="26"/>
+      <c r="M87" s="39"/>
+      <c r="N87" s="40"/>
+      <c r="O87" s="40"/>
+      <c r="P87" s="40"/>
+      <c r="Q87" s="41"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A88" s="9">
@@ -4927,11 +4931,11 @@
         <f t="shared" si="6"/>
         <v>0.42949999999999999</v>
       </c>
-      <c r="M88" s="24"/>
-      <c r="N88" s="25"/>
-      <c r="O88" s="25"/>
-      <c r="P88" s="25"/>
-      <c r="Q88" s="26"/>
+      <c r="M88" s="39"/>
+      <c r="N88" s="40"/>
+      <c r="O88" s="40"/>
+      <c r="P88" s="40"/>
+      <c r="Q88" s="41"/>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A89" s="9">
@@ -4969,11 +4973,11 @@
         <f t="shared" si="6"/>
         <v>0.44424999999999998</v>
       </c>
-      <c r="M89" s="24"/>
-      <c r="N89" s="25"/>
-      <c r="O89" s="25"/>
-      <c r="P89" s="25"/>
-      <c r="Q89" s="26"/>
+      <c r="M89" s="39"/>
+      <c r="N89" s="40"/>
+      <c r="O89" s="40"/>
+      <c r="P89" s="40"/>
+      <c r="Q89" s="41"/>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A90" s="9">
@@ -5011,11 +5015,11 @@
         <f t="shared" si="6"/>
         <v>0.30775000000000002</v>
       </c>
-      <c r="M90" s="24"/>
-      <c r="N90" s="25"/>
-      <c r="O90" s="25"/>
-      <c r="P90" s="25"/>
-      <c r="Q90" s="26"/>
+      <c r="M90" s="39"/>
+      <c r="N90" s="40"/>
+      <c r="O90" s="40"/>
+      <c r="P90" s="40"/>
+      <c r="Q90" s="41"/>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A91" s="9">
@@ -5053,11 +5057,11 @@
         <f t="shared" si="6"/>
         <v>0.42512499999999998</v>
       </c>
-      <c r="M91" s="24"/>
-      <c r="N91" s="25"/>
-      <c r="O91" s="25"/>
-      <c r="P91" s="25"/>
-      <c r="Q91" s="26"/>
+      <c r="M91" s="39"/>
+      <c r="N91" s="40"/>
+      <c r="O91" s="40"/>
+      <c r="P91" s="40"/>
+      <c r="Q91" s="41"/>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A92" s="9">
@@ -5095,11 +5099,11 @@
         <f t="shared" si="6"/>
         <v>0.64700000000000002</v>
       </c>
-      <c r="M92" s="24"/>
-      <c r="N92" s="25"/>
-      <c r="O92" s="25"/>
-      <c r="P92" s="25"/>
-      <c r="Q92" s="26"/>
+      <c r="M92" s="39"/>
+      <c r="N92" s="40"/>
+      <c r="O92" s="40"/>
+      <c r="P92" s="40"/>
+      <c r="Q92" s="41"/>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A93" s="9">
@@ -5137,11 +5141,11 @@
         <f t="shared" si="6"/>
         <v>0.43662499999999999</v>
       </c>
-      <c r="M93" s="24"/>
-      <c r="N93" s="25"/>
-      <c r="O93" s="25"/>
-      <c r="P93" s="25"/>
-      <c r="Q93" s="26"/>
+      <c r="M93" s="39"/>
+      <c r="N93" s="40"/>
+      <c r="O93" s="40"/>
+      <c r="P93" s="40"/>
+      <c r="Q93" s="41"/>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A94" s="9">
@@ -5179,11 +5183,11 @@
         <f t="shared" si="6"/>
         <v>0.31337500000000001</v>
       </c>
-      <c r="M94" s="24"/>
-      <c r="N94" s="25"/>
-      <c r="O94" s="25"/>
-      <c r="P94" s="25"/>
-      <c r="Q94" s="26"/>
+      <c r="M94" s="39"/>
+      <c r="N94" s="40"/>
+      <c r="O94" s="40"/>
+      <c r="P94" s="40"/>
+      <c r="Q94" s="41"/>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A95" s="9">
@@ -5221,11 +5225,11 @@
         <f t="shared" si="6"/>
         <v>0.49612499999999998</v>
       </c>
-      <c r="M95" s="24"/>
-      <c r="N95" s="25"/>
-      <c r="O95" s="25"/>
-      <c r="P95" s="25"/>
-      <c r="Q95" s="26"/>
+      <c r="M95" s="39"/>
+      <c r="N95" s="40"/>
+      <c r="O95" s="40"/>
+      <c r="P95" s="40"/>
+      <c r="Q95" s="41"/>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A96" s="9">
@@ -5263,11 +5267,11 @@
         <f t="shared" si="6"/>
         <v>0.43049999999999999</v>
       </c>
-      <c r="M96" s="24"/>
-      <c r="N96" s="25"/>
-      <c r="O96" s="25"/>
-      <c r="P96" s="25"/>
-      <c r="Q96" s="26"/>
+      <c r="M96" s="39"/>
+      <c r="N96" s="40"/>
+      <c r="O96" s="40"/>
+      <c r="P96" s="40"/>
+      <c r="Q96" s="41"/>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A97" s="9">
@@ -5305,11 +5309,11 @@
         <f t="shared" si="6"/>
         <v>0.608375</v>
       </c>
-      <c r="M97" s="24"/>
-      <c r="N97" s="25"/>
-      <c r="O97" s="25"/>
-      <c r="P97" s="25"/>
-      <c r="Q97" s="26"/>
+      <c r="M97" s="39"/>
+      <c r="N97" s="40"/>
+      <c r="O97" s="40"/>
+      <c r="P97" s="40"/>
+      <c r="Q97" s="41"/>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A98" s="9">
@@ -5347,11 +5351,11 @@
         <f t="shared" si="6"/>
         <v>0.455125</v>
       </c>
-      <c r="M98" s="27"/>
-      <c r="N98" s="28"/>
-      <c r="O98" s="28"/>
-      <c r="P98" s="28"/>
-      <c r="Q98" s="29"/>
+      <c r="M98" s="42"/>
+      <c r="N98" s="43"/>
+      <c r="O98" s="43"/>
+      <c r="P98" s="43"/>
+      <c r="Q98" s="44"/>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A99" s="9">
@@ -5426,13 +5430,13 @@
         <f t="shared" si="6"/>
         <v>0.41962500000000003</v>
       </c>
-      <c r="M100" s="21" t="s">
+      <c r="M100" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="N100" s="22"/>
-      <c r="O100" s="22"/>
-      <c r="P100" s="22"/>
-      <c r="Q100" s="23"/>
+      <c r="N100" s="49"/>
+      <c r="O100" s="49"/>
+      <c r="P100" s="49"/>
+      <c r="Q100" s="50"/>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A101" s="9">
@@ -5470,11 +5474,11 @@
         <f t="shared" si="6"/>
         <v>0.2185</v>
       </c>
-      <c r="M101" s="24"/>
-      <c r="N101" s="25"/>
-      <c r="O101" s="25"/>
-      <c r="P101" s="25"/>
-      <c r="Q101" s="26"/>
+      <c r="M101" s="39"/>
+      <c r="N101" s="40"/>
+      <c r="O101" s="40"/>
+      <c r="P101" s="40"/>
+      <c r="Q101" s="41"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A102" s="9">
@@ -5512,11 +5516,11 @@
         <f t="shared" si="6"/>
         <v>0.417875</v>
       </c>
-      <c r="M102" s="24"/>
-      <c r="N102" s="25"/>
-      <c r="O102" s="25"/>
-      <c r="P102" s="25"/>
-      <c r="Q102" s="26"/>
+      <c r="M102" s="39"/>
+      <c r="N102" s="40"/>
+      <c r="O102" s="40"/>
+      <c r="P102" s="40"/>
+      <c r="Q102" s="41"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A103" s="9">
@@ -5554,11 +5558,11 @@
         <f t="shared" si="6"/>
         <v>0.390125</v>
       </c>
-      <c r="M103" s="24"/>
-      <c r="N103" s="25"/>
-      <c r="O103" s="25"/>
-      <c r="P103" s="25"/>
-      <c r="Q103" s="26"/>
+      <c r="M103" s="39"/>
+      <c r="N103" s="40"/>
+      <c r="O103" s="40"/>
+      <c r="P103" s="40"/>
+      <c r="Q103" s="41"/>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A104" s="9">
@@ -5596,11 +5600,11 @@
         <f t="shared" si="6"/>
         <v>0.32887499999999997</v>
       </c>
-      <c r="M104" s="24"/>
-      <c r="N104" s="25"/>
-      <c r="O104" s="25"/>
-      <c r="P104" s="25"/>
-      <c r="Q104" s="26"/>
+      <c r="M104" s="39"/>
+      <c r="N104" s="40"/>
+      <c r="O104" s="40"/>
+      <c r="P104" s="40"/>
+      <c r="Q104" s="41"/>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A105" s="9">
@@ -5638,11 +5642,11 @@
         <f t="shared" si="6"/>
         <v>0.43087500000000001</v>
       </c>
-      <c r="M105" s="24"/>
-      <c r="N105" s="25"/>
-      <c r="O105" s="25"/>
-      <c r="P105" s="25"/>
-      <c r="Q105" s="26"/>
+      <c r="M105" s="39"/>
+      <c r="N105" s="40"/>
+      <c r="O105" s="40"/>
+      <c r="P105" s="40"/>
+      <c r="Q105" s="41"/>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A106" s="9">
@@ -5680,11 +5684,11 @@
         <f t="shared" si="6"/>
         <v>0.40987499999999999</v>
       </c>
-      <c r="M106" s="24"/>
-      <c r="N106" s="25"/>
-      <c r="O106" s="25"/>
-      <c r="P106" s="25"/>
-      <c r="Q106" s="26"/>
+      <c r="M106" s="39"/>
+      <c r="N106" s="40"/>
+      <c r="O106" s="40"/>
+      <c r="P106" s="40"/>
+      <c r="Q106" s="41"/>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A107" s="9">
@@ -5722,11 +5726,11 @@
         <f t="shared" si="6"/>
         <v>0.45687499999999998</v>
       </c>
-      <c r="M107" s="24"/>
-      <c r="N107" s="25"/>
-      <c r="O107" s="25"/>
-      <c r="P107" s="25"/>
-      <c r="Q107" s="26"/>
+      <c r="M107" s="39"/>
+      <c r="N107" s="40"/>
+      <c r="O107" s="40"/>
+      <c r="P107" s="40"/>
+      <c r="Q107" s="41"/>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A108" s="9">
@@ -5764,11 +5768,11 @@
         <f t="shared" si="6"/>
         <v>0.324125</v>
       </c>
-      <c r="M108" s="24"/>
-      <c r="N108" s="25"/>
-      <c r="O108" s="25"/>
-      <c r="P108" s="25"/>
-      <c r="Q108" s="26"/>
+      <c r="M108" s="39"/>
+      <c r="N108" s="40"/>
+      <c r="O108" s="40"/>
+      <c r="P108" s="40"/>
+      <c r="Q108" s="41"/>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A109" s="9">
@@ -5806,11 +5810,11 @@
         <f t="shared" si="6"/>
         <v>0.439</v>
       </c>
-      <c r="M109" s="24"/>
-      <c r="N109" s="25"/>
-      <c r="O109" s="25"/>
-      <c r="P109" s="25"/>
-      <c r="Q109" s="26"/>
+      <c r="M109" s="39"/>
+      <c r="N109" s="40"/>
+      <c r="O109" s="40"/>
+      <c r="P109" s="40"/>
+      <c r="Q109" s="41"/>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A110" s="9">
@@ -5848,11 +5852,11 @@
         <f t="shared" si="6"/>
         <v>0.51512500000000006</v>
       </c>
-      <c r="M110" s="24"/>
-      <c r="N110" s="25"/>
-      <c r="O110" s="25"/>
-      <c r="P110" s="25"/>
-      <c r="Q110" s="26"/>
+      <c r="M110" s="39"/>
+      <c r="N110" s="40"/>
+      <c r="O110" s="40"/>
+      <c r="P110" s="40"/>
+      <c r="Q110" s="41"/>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A111" s="9">
@@ -5890,11 +5894,11 @@
         <f t="shared" si="6"/>
         <v>0.332125</v>
       </c>
-      <c r="M111" s="24"/>
-      <c r="N111" s="25"/>
-      <c r="O111" s="25"/>
-      <c r="P111" s="25"/>
-      <c r="Q111" s="26"/>
+      <c r="M111" s="39"/>
+      <c r="N111" s="40"/>
+      <c r="O111" s="40"/>
+      <c r="P111" s="40"/>
+      <c r="Q111" s="41"/>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A112" s="9">
@@ -5932,11 +5936,11 @@
         <f t="shared" si="6"/>
         <v>0.41699999999999998</v>
       </c>
-      <c r="M112" s="24"/>
-      <c r="N112" s="25"/>
-      <c r="O112" s="25"/>
-      <c r="P112" s="25"/>
-      <c r="Q112" s="26"/>
+      <c r="M112" s="39"/>
+      <c r="N112" s="40"/>
+      <c r="O112" s="40"/>
+      <c r="P112" s="40"/>
+      <c r="Q112" s="41"/>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A113" s="9">
@@ -5974,11 +5978,11 @@
         <f t="shared" si="6"/>
         <v>0.42925000000000002</v>
       </c>
-      <c r="M113" s="24"/>
-      <c r="N113" s="25"/>
-      <c r="O113" s="25"/>
-      <c r="P113" s="25"/>
-      <c r="Q113" s="26"/>
+      <c r="M113" s="39"/>
+      <c r="N113" s="40"/>
+      <c r="O113" s="40"/>
+      <c r="P113" s="40"/>
+      <c r="Q113" s="41"/>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A114" s="9">
@@ -6016,11 +6020,11 @@
         <f t="shared" si="6"/>
         <v>0.41649999999999998</v>
       </c>
-      <c r="M114" s="24"/>
-      <c r="N114" s="25"/>
-      <c r="O114" s="25"/>
-      <c r="P114" s="25"/>
-      <c r="Q114" s="26"/>
+      <c r="M114" s="39"/>
+      <c r="N114" s="40"/>
+      <c r="O114" s="40"/>
+      <c r="P114" s="40"/>
+      <c r="Q114" s="41"/>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A115" s="9">
@@ -6058,11 +6062,11 @@
         <f t="shared" si="6"/>
         <v>0.442</v>
       </c>
-      <c r="M115" s="24"/>
-      <c r="N115" s="25"/>
-      <c r="O115" s="25"/>
-      <c r="P115" s="25"/>
-      <c r="Q115" s="26"/>
+      <c r="M115" s="39"/>
+      <c r="N115" s="40"/>
+      <c r="O115" s="40"/>
+      <c r="P115" s="40"/>
+      <c r="Q115" s="41"/>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A116" s="9">
@@ -6100,11 +6104,11 @@
         <f t="shared" si="6"/>
         <v>0.43837500000000001</v>
       </c>
-      <c r="M116" s="27"/>
-      <c r="N116" s="28"/>
-      <c r="O116" s="28"/>
-      <c r="P116" s="28"/>
-      <c r="Q116" s="29"/>
+      <c r="M116" s="42"/>
+      <c r="N116" s="43"/>
+      <c r="O116" s="43"/>
+      <c r="P116" s="43"/>
+      <c r="Q116" s="44"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A117" s="9">
@@ -6179,13 +6183,13 @@
         <f t="shared" si="6"/>
         <v>0.42525000000000002</v>
       </c>
-      <c r="M118" s="51" t="s">
+      <c r="M118" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="N118" s="51"/>
-      <c r="O118" s="51"/>
-      <c r="P118" s="51"/>
-      <c r="Q118" s="51"/>
+      <c r="N118" s="38"/>
+      <c r="O118" s="38"/>
+      <c r="P118" s="38"/>
+      <c r="Q118" s="38"/>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A119" s="9">
@@ -6223,13 +6227,13 @@
         <f t="shared" si="6"/>
         <v>0.44237500000000002</v>
       </c>
-      <c r="M119" s="51" t="s">
+      <c r="M119" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="N119" s="51"/>
-      <c r="O119" s="51"/>
-      <c r="P119" s="51"/>
-      <c r="Q119" s="51"/>
+      <c r="N119" s="38"/>
+      <c r="O119" s="38"/>
+      <c r="P119" s="38"/>
+      <c r="Q119" s="38"/>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A120" s="9">
@@ -6267,13 +6271,13 @@
         <f t="shared" si="6"/>
         <v>0.333625</v>
       </c>
-      <c r="M120" s="51" t="s">
+      <c r="M120" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="N120" s="51"/>
-      <c r="O120" s="51"/>
-      <c r="P120" s="51"/>
-      <c r="Q120" s="51"/>
+      <c r="N120" s="38"/>
+      <c r="O120" s="38"/>
+      <c r="P120" s="38"/>
+      <c r="Q120" s="38"/>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A121" s="9">
@@ -6311,6 +6315,13 @@
         <f t="shared" si="6"/>
         <v>0.44137500000000002</v>
       </c>
+      <c r="M121" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="N121" s="38"/>
+      <c r="O121" s="38"/>
+      <c r="P121" s="38"/>
+      <c r="Q121" s="38"/>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A122" s="9">
@@ -24080,38 +24091,38 @@
       <c r="B603" s="9">
         <v>6</v>
       </c>
-      <c r="C603" s="39" t="s">
+      <c r="C603" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="D603" s="40">
+      <c r="D603" s="29">
         <f>AVERAGEIFS(D$2:D$601, $A$2:$A$601, $A603, $B$2:$B$601, $B603)</f>
         <v>3.5350599999999996</v>
       </c>
-      <c r="E603" s="40">
+      <c r="E603" s="29">
         <f t="shared" ref="E603:K608" si="23">AVERAGEIFS(E$2:E$601, $A$2:$A$601, $A603, $B$2:$B$601, $B603)</f>
         <v>3.4874900000000006</v>
       </c>
-      <c r="F603" s="41">
+      <c r="F603" s="30">
         <f t="shared" si="23"/>
         <v>0.9329572364663733</v>
       </c>
-      <c r="G603" s="42">
+      <c r="G603" s="31">
         <f t="shared" si="23"/>
         <v>1.0221349999999995E-2</v>
       </c>
-      <c r="H603" s="42">
+      <c r="H603" s="31">
         <f t="shared" si="23"/>
         <v>1.084164E-2</v>
       </c>
-      <c r="I603" s="43">
+      <c r="I603" s="32">
         <f t="shared" si="23"/>
         <v>99.866831179999991</v>
       </c>
-      <c r="J603" s="44">
+      <c r="J603" s="33">
         <f t="shared" si="23"/>
         <v>0.44188249999999996</v>
       </c>
-      <c r="K603" s="44">
+      <c r="K603" s="33">
         <f t="shared" si="23"/>
         <v>0.43593625000000008</v>
       </c>
@@ -24123,36 +24134,36 @@
       <c r="B604" s="9">
         <v>10</v>
       </c>
-      <c r="C604" s="39"/>
-      <c r="D604" s="40">
+      <c r="C604" s="51"/>
+      <c r="D604" s="29">
         <f t="shared" ref="D604:D608" si="24">AVERAGEIFS(D$2:D$601, $A$2:$A$601, $A604, $B$2:$B$601, $B604)</f>
         <v>3.4885200000000021</v>
       </c>
-      <c r="E604" s="40">
+      <c r="E604" s="29">
         <f t="shared" si="23"/>
         <v>3.4284600000000016</v>
       </c>
-      <c r="F604" s="41">
+      <c r="F604" s="30">
         <f t="shared" si="23"/>
         <v>0.92011603696679656</v>
       </c>
-      <c r="G604" s="42">
+      <c r="G604" s="31">
         <f t="shared" si="23"/>
         <v>6.8845099999999991E-3</v>
       </c>
-      <c r="H604" s="42">
+      <c r="H604" s="31">
         <f t="shared" si="23"/>
         <v>6.8512799999999978E-3</v>
       </c>
-      <c r="I604" s="43">
+      <c r="I604" s="32">
         <f t="shared" si="23"/>
         <v>100.96643069</v>
       </c>
-      <c r="J604" s="44">
+      <c r="J604" s="33">
         <f t="shared" si="23"/>
         <v>0.43606500000000026</v>
       </c>
-      <c r="K604" s="44">
+      <c r="K604" s="33">
         <f t="shared" si="23"/>
         <v>0.4285575000000002</v>
       </c>
@@ -24164,36 +24175,36 @@
       <c r="B605" s="9">
         <v>6</v>
       </c>
-      <c r="C605" s="39"/>
-      <c r="D605" s="40">
+      <c r="C605" s="51"/>
+      <c r="D605" s="29">
         <f t="shared" si="24"/>
         <v>5.5705100000000023</v>
       </c>
-      <c r="E605" s="40">
+      <c r="E605" s="29">
         <f t="shared" si="23"/>
         <v>5.3169200000000023</v>
       </c>
-      <c r="F605" s="41">
+      <c r="F605" s="30">
         <f t="shared" si="23"/>
         <v>0.95658884767965546</v>
       </c>
-      <c r="G605" s="42">
+      <c r="G605" s="31">
         <f t="shared" si="23"/>
         <v>2.5650999999999994E-3</v>
       </c>
-      <c r="H605" s="42">
+      <c r="H605" s="31">
         <f t="shared" si="23"/>
         <v>2.950599999999999E-3</v>
       </c>
-      <c r="I605" s="43">
+      <c r="I605" s="32">
         <f t="shared" si="23"/>
         <v>90.980326890000001</v>
       </c>
-      <c r="J605" s="44">
+      <c r="J605" s="33">
         <f t="shared" si="23"/>
         <v>0.46420916666666656</v>
       </c>
-      <c r="K605" s="44">
+      <c r="K605" s="33">
         <f t="shared" si="23"/>
         <v>0.44307666666666662</v>
       </c>
@@ -24205,36 +24216,36 @@
       <c r="B606" s="9">
         <v>10</v>
       </c>
-      <c r="C606" s="39"/>
-      <c r="D606" s="40">
+      <c r="C606" s="51"/>
+      <c r="D606" s="29">
         <f t="shared" si="24"/>
         <v>5.5629699999999982</v>
       </c>
-      <c r="E606" s="40">
+      <c r="E606" s="29">
         <f t="shared" si="23"/>
         <v>5.5734000000000012</v>
       </c>
-      <c r="F606" s="41">
+      <c r="F606" s="30">
         <f t="shared" si="23"/>
         <v>0.95034614942020257</v>
       </c>
-      <c r="G606" s="42">
+      <c r="G606" s="31">
         <f t="shared" si="23"/>
         <v>1.6486999999999997E-3</v>
       </c>
-      <c r="H606" s="42">
+      <c r="H606" s="31">
         <f t="shared" si="23"/>
         <v>1.7895599999999997E-3</v>
       </c>
-      <c r="I606" s="43">
+      <c r="I606" s="32">
         <f t="shared" si="23"/>
         <v>93.968004070000006</v>
       </c>
-      <c r="J606" s="44">
+      <c r="J606" s="33">
         <f t="shared" si="23"/>
         <v>0.46358083333333355</v>
       </c>
-      <c r="K606" s="44">
+      <c r="K606" s="33">
         <f t="shared" si="23"/>
         <v>0.46445000000000003</v>
       </c>
@@ -24246,36 +24257,36 @@
       <c r="B607" s="9">
         <v>6</v>
       </c>
-      <c r="C607" s="39"/>
-      <c r="D607" s="40">
+      <c r="C607" s="51"/>
+      <c r="D607" s="29">
         <f t="shared" si="24"/>
         <v>7.4428200000000002</v>
       </c>
-      <c r="E607" s="40">
+      <c r="E607" s="29">
         <f t="shared" si="23"/>
         <v>7.4438899999999979</v>
       </c>
-      <c r="F607" s="41">
+      <c r="F607" s="30">
         <f t="shared" si="23"/>
         <v>0.96854184419386702</v>
       </c>
-      <c r="G607" s="42">
+      <c r="G607" s="31">
         <f t="shared" si="23"/>
         <v>7.8936999999999953E-4</v>
       </c>
-      <c r="H607" s="42">
+      <c r="H607" s="31">
         <f t="shared" si="23"/>
         <v>9.935800000000002E-4</v>
       </c>
-      <c r="I607" s="43">
+      <c r="I607" s="32">
         <f t="shared" si="23"/>
         <v>85.409989529999962</v>
       </c>
-      <c r="J607" s="44">
+      <c r="J607" s="33">
         <f t="shared" si="23"/>
         <v>0.46517625000000001</v>
       </c>
-      <c r="K607" s="44">
+      <c r="K607" s="33">
         <f t="shared" si="23"/>
         <v>0.46524312499999987</v>
       </c>
@@ -24287,47 +24298,47 @@
       <c r="B608" s="9">
         <v>10</v>
       </c>
-      <c r="C608" s="39"/>
-      <c r="D608" s="40">
+      <c r="C608" s="51"/>
+      <c r="D608" s="29">
         <f t="shared" si="24"/>
         <v>7.4845899999999972</v>
       </c>
-      <c r="E608" s="40">
+      <c r="E608" s="29">
         <f t="shared" si="23"/>
         <v>7.5141200000000019</v>
       </c>
-      <c r="F608" s="41">
+      <c r="F608" s="30">
         <f t="shared" si="23"/>
         <v>0.96273261843184077</v>
       </c>
-      <c r="G608" s="42">
+      <c r="G608" s="31">
         <f t="shared" si="23"/>
         <v>5.2996000000000011E-4</v>
       </c>
-      <c r="H608" s="42">
+      <c r="H608" s="31">
         <f t="shared" si="23"/>
         <v>5.8561999999999959E-4</v>
       </c>
-      <c r="I608" s="43">
+      <c r="I608" s="32">
         <f t="shared" si="23"/>
         <v>92.147266639999941</v>
       </c>
-      <c r="J608" s="44">
+      <c r="J608" s="33">
         <f t="shared" si="23"/>
         <v>0.46778687499999982</v>
       </c>
-      <c r="K608" s="44">
+      <c r="K608" s="33">
         <f t="shared" si="23"/>
         <v>0.46963250000000012</v>
       </c>
     </row>
     <row r="609" spans="1:11" ht="8.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D609" s="30"/>
-      <c r="E609" s="30"/>
-      <c r="F609" s="31"/>
-      <c r="I609" s="32"/>
-      <c r="J609" s="32"/>
-      <c r="K609" s="32"/>
+      <c r="D609" s="21"/>
+      <c r="E609" s="21"/>
+      <c r="F609" s="22"/>
+      <c r="I609" s="23"/>
+      <c r="J609" s="23"/>
+      <c r="K609" s="23"/>
     </row>
     <row r="610" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A610" s="9">
@@ -24336,38 +24347,38 @@
       <c r="B610" s="9">
         <v>6</v>
       </c>
-      <c r="C610" s="38" t="s">
+      <c r="C610" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="D610" s="33">
+      <c r="D610" s="24">
         <f>_xlfn.STDEV.P(D2:D101)</f>
         <v>0.59371420431045641</v>
       </c>
-      <c r="E610" s="33">
+      <c r="E610" s="24">
         <f t="shared" ref="E610:K610" si="25">_xlfn.STDEV.P(E2:E101)</f>
         <v>0.73044200995013631</v>
       </c>
-      <c r="F610" s="34">
+      <c r="F610" s="25">
         <f t="shared" si="25"/>
         <v>1.2228688797035175E-2</v>
       </c>
-      <c r="G610" s="35">
+      <c r="G610" s="26">
         <f t="shared" si="25"/>
         <v>4.3100882992695337E-3</v>
       </c>
-      <c r="H610" s="35">
+      <c r="H610" s="26">
         <f t="shared" si="25"/>
         <v>6.9818874002951312E-3</v>
       </c>
-      <c r="I610" s="36">
+      <c r="I610" s="27">
         <f t="shared" si="25"/>
         <v>18.101097411295623</v>
       </c>
-      <c r="J610" s="37">
+      <c r="J610" s="28">
         <f t="shared" si="25"/>
         <v>7.4214275538807051E-2</v>
       </c>
-      <c r="K610" s="37">
+      <c r="K610" s="28">
         <f t="shared" si="25"/>
         <v>9.1305251243767038E-2</v>
       </c>
@@ -24379,36 +24390,36 @@
       <c r="B611" s="9">
         <v>10</v>
       </c>
-      <c r="C611" s="38"/>
-      <c r="D611" s="33">
+      <c r="C611" s="45"/>
+      <c r="D611" s="24">
         <f>_xlfn.STDEV.P(D102:D201)</f>
         <v>0.46697866075441075</v>
       </c>
-      <c r="E611" s="33">
+      <c r="E611" s="24">
         <f t="shared" ref="E611:K611" si="26">_xlfn.STDEV.P(E102:E201)</f>
         <v>0.44034289865966075</v>
       </c>
-      <c r="F611" s="34">
+      <c r="F611" s="25">
         <f t="shared" si="26"/>
         <v>1.1256060304962434E-2</v>
       </c>
-      <c r="G611" s="35">
+      <c r="G611" s="26">
         <f t="shared" si="26"/>
         <v>2.1864792086594377E-3</v>
       </c>
-      <c r="H611" s="35">
+      <c r="H611" s="26">
         <f t="shared" si="26"/>
         <v>2.051644828326774E-3</v>
       </c>
-      <c r="I611" s="36">
+      <c r="I611" s="27">
         <f t="shared" si="26"/>
         <v>14.688874013233969</v>
       </c>
-      <c r="J611" s="37">
+      <c r="J611" s="28">
         <f t="shared" si="26"/>
         <v>5.8372332594301343E-2</v>
       </c>
-      <c r="K611" s="37">
+      <c r="K611" s="28">
         <f t="shared" si="26"/>
         <v>5.5042862332457594E-2</v>
       </c>
@@ -24420,36 +24431,36 @@
       <c r="B612" s="9">
         <v>6</v>
       </c>
-      <c r="C612" s="38"/>
-      <c r="D612" s="33">
+      <c r="C612" s="45"/>
+      <c r="D612" s="24">
         <f>_xlfn.STDEV.P(D202:D301)</f>
         <v>1.0813968420057296</v>
       </c>
-      <c r="E612" s="33">
+      <c r="E612" s="24">
         <f t="shared" ref="E612:K612" si="27">_xlfn.STDEV.P(E202:E301)</f>
         <v>0.99417799895188974</v>
       </c>
-      <c r="F612" s="34">
+      <c r="F612" s="25">
         <f t="shared" si="27"/>
         <v>6.8481711319464461E-3</v>
       </c>
-      <c r="G612" s="35">
+      <c r="G612" s="26">
         <f t="shared" si="27"/>
         <v>1.41015056997471E-3</v>
       </c>
-      <c r="H612" s="35">
+      <c r="H612" s="26">
         <f t="shared" si="27"/>
         <v>1.7935342093196895E-3</v>
       </c>
-      <c r="I612" s="36">
+      <c r="I612" s="27">
         <f t="shared" si="27"/>
         <v>17.316336117647388</v>
       </c>
-      <c r="J612" s="37">
+      <c r="J612" s="28">
         <f t="shared" si="27"/>
         <v>9.0116403500478892E-2</v>
       </c>
-      <c r="K612" s="37">
+      <c r="K612" s="28">
         <f t="shared" si="27"/>
         <v>8.2848166579325269E-2</v>
       </c>
@@ -24461,36 +24472,36 @@
       <c r="B613" s="9">
         <v>10</v>
       </c>
-      <c r="C613" s="38"/>
-      <c r="D613" s="33">
+      <c r="C613" s="45"/>
+      <c r="D613" s="24">
         <f>_xlfn.STDEV.P(D302:D401)</f>
         <v>0.61227971475464116</v>
       </c>
-      <c r="E613" s="33">
+      <c r="E613" s="24">
         <f t="shared" ref="E613:K613" si="28">_xlfn.STDEV.P(E302:E401)</f>
         <v>0.74032754912942444</v>
       </c>
-      <c r="F613" s="34">
+      <c r="F613" s="25">
         <f t="shared" si="28"/>
         <v>7.2804720840312417E-3</v>
       </c>
-      <c r="G613" s="35">
+      <c r="G613" s="26">
         <f t="shared" si="28"/>
         <v>6.3073476993107016E-4</v>
       </c>
-      <c r="H613" s="35">
+      <c r="H613" s="26">
         <f t="shared" si="28"/>
         <v>7.534120827276397E-4</v>
       </c>
-      <c r="I613" s="36">
+      <c r="I613" s="27">
         <f t="shared" si="28"/>
         <v>13.985795705348458</v>
       </c>
-      <c r="J613" s="37">
+      <c r="J613" s="28">
         <f t="shared" si="28"/>
         <v>5.1023309562881668E-2</v>
       </c>
-      <c r="K613" s="37">
+      <c r="K613" s="28">
         <f t="shared" si="28"/>
         <v>6.1693962427453265E-2</v>
       </c>
@@ -24502,36 +24513,36 @@
       <c r="B614" s="9">
         <v>6</v>
       </c>
-      <c r="C614" s="38"/>
-      <c r="D614" s="33">
+      <c r="C614" s="45"/>
+      <c r="D614" s="24">
         <f>_xlfn.STDEV.P(D402:D501)</f>
         <v>1.3270620586845225</v>
       </c>
-      <c r="E614" s="33">
+      <c r="E614" s="24">
         <f t="shared" ref="E614:K614" si="29">_xlfn.STDEV.P(E402:E501)</f>
         <v>1.6319948706720979</v>
       </c>
-      <c r="F614" s="34">
+      <c r="F614" s="25">
         <f t="shared" si="29"/>
         <v>4.2375500880114866E-3</v>
       </c>
-      <c r="G614" s="35">
+      <c r="G614" s="26">
         <f t="shared" si="29"/>
         <v>4.2207083895952829E-4</v>
       </c>
-      <c r="H614" s="35">
+      <c r="H614" s="26">
         <f t="shared" si="29"/>
         <v>6.1986400411703215E-4</v>
       </c>
-      <c r="I614" s="36">
+      <c r="I614" s="27">
         <f t="shared" si="29"/>
         <v>18.929898461726527</v>
       </c>
-      <c r="J614" s="37">
+      <c r="J614" s="28">
         <f t="shared" si="29"/>
         <v>8.2941378667782659E-2</v>
       </c>
-      <c r="K614" s="37">
+      <c r="K614" s="28">
         <f t="shared" si="29"/>
         <v>0.10199967941700612</v>
       </c>
@@ -24543,36 +24554,36 @@
       <c r="B615" s="9">
         <v>10</v>
       </c>
-      <c r="C615" s="38"/>
-      <c r="D615" s="33">
+      <c r="C615" s="45"/>
+      <c r="D615" s="24">
         <f>_xlfn.STDEV.P(D502:D601)</f>
         <v>0.83248367065068873</v>
       </c>
-      <c r="E615" s="33">
+      <c r="E615" s="24">
         <f t="shared" ref="E615:K615" si="30">_xlfn.STDEV.P(E502:E601)</f>
         <v>0.89260305040929844</v>
       </c>
-      <c r="F615" s="34">
+      <c r="F615" s="25">
         <f t="shared" si="30"/>
         <v>3.4889624396273601E-3</v>
       </c>
-      <c r="G615" s="35">
+      <c r="G615" s="26">
         <f t="shared" si="30"/>
         <v>2.1433580755440747E-4</v>
       </c>
-      <c r="H615" s="35">
+      <c r="H615" s="26">
         <f t="shared" si="30"/>
         <v>2.508201259867318E-4</v>
       </c>
-      <c r="I615" s="36">
+      <c r="I615" s="27">
         <f t="shared" si="30"/>
         <v>13.492242420852939</v>
       </c>
-      <c r="J615" s="37">
+      <c r="J615" s="28">
         <f t="shared" si="30"/>
         <v>5.2030229415668046E-2</v>
       </c>
-      <c r="K615" s="37">
+      <c r="K615" s="28">
         <f t="shared" si="30"/>
         <v>5.5787690650581152E-2</v>
       </c>
@@ -24585,38 +24596,38 @@
       <c r="B617" s="9">
         <v>6</v>
       </c>
-      <c r="C617" s="38" t="s">
+      <c r="C617" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="D617" s="40">
+      <c r="D617" s="29">
         <f>D610/10</f>
         <v>5.9371420431045638E-2</v>
       </c>
-      <c r="E617" s="40">
+      <c r="E617" s="29">
         <f t="shared" ref="E617:K617" si="31">E610/10</f>
         <v>7.3044200995013631E-2</v>
       </c>
-      <c r="F617" s="41">
+      <c r="F617" s="30">
         <f t="shared" si="31"/>
         <v>1.2228688797035175E-3</v>
       </c>
-      <c r="G617" s="42">
+      <c r="G617" s="31">
         <f t="shared" si="31"/>
         <v>4.3100882992695336E-4</v>
       </c>
-      <c r="H617" s="42">
+      <c r="H617" s="31">
         <f t="shared" si="31"/>
         <v>6.9818874002951312E-4</v>
       </c>
-      <c r="I617" s="43">
+      <c r="I617" s="32">
         <f t="shared" si="31"/>
         <v>1.8101097411295624</v>
       </c>
-      <c r="J617" s="44">
+      <c r="J617" s="33">
         <f t="shared" si="31"/>
         <v>7.4214275538807047E-3</v>
       </c>
-      <c r="K617" s="44">
+      <c r="K617" s="33">
         <f t="shared" si="31"/>
         <v>9.1305251243767038E-3</v>
       </c>
@@ -24628,36 +24639,36 @@
       <c r="B618" s="9">
         <v>10</v>
       </c>
-      <c r="C618" s="38"/>
-      <c r="D618" s="40">
+      <c r="C618" s="45"/>
+      <c r="D618" s="29">
         <f t="shared" ref="D618:K618" si="32">D611/10</f>
         <v>4.6697866075441075E-2</v>
       </c>
-      <c r="E618" s="40">
+      <c r="E618" s="29">
         <f t="shared" si="32"/>
         <v>4.4034289865966074E-2</v>
       </c>
-      <c r="F618" s="41">
+      <c r="F618" s="30">
         <f t="shared" si="32"/>
         <v>1.1256060304962435E-3</v>
       </c>
-      <c r="G618" s="42">
+      <c r="G618" s="31">
         <f t="shared" si="32"/>
         <v>2.1864792086594376E-4</v>
       </c>
-      <c r="H618" s="42">
+      <c r="H618" s="31">
         <f t="shared" si="32"/>
         <v>2.0516448283267741E-4</v>
       </c>
-      <c r="I618" s="43">
+      <c r="I618" s="32">
         <f t="shared" si="32"/>
         <v>1.4688874013233968</v>
       </c>
-      <c r="J618" s="44">
+      <c r="J618" s="33">
         <f t="shared" si="32"/>
         <v>5.8372332594301343E-3</v>
       </c>
-      <c r="K618" s="44">
+      <c r="K618" s="33">
         <f t="shared" si="32"/>
         <v>5.5042862332457592E-3</v>
       </c>
@@ -24669,36 +24680,36 @@
       <c r="B619" s="9">
         <v>6</v>
       </c>
-      <c r="C619" s="38"/>
-      <c r="D619" s="40">
+      <c r="C619" s="45"/>
+      <c r="D619" s="29">
         <f t="shared" ref="D619:K619" si="33">D612/10</f>
         <v>0.10813968420057296</v>
       </c>
-      <c r="E619" s="40">
+      <c r="E619" s="29">
         <f t="shared" si="33"/>
         <v>9.941779989518898E-2</v>
       </c>
-      <c r="F619" s="41">
+      <c r="F619" s="30">
         <f t="shared" si="33"/>
         <v>6.8481711319464463E-4</v>
       </c>
-      <c r="G619" s="42">
+      <c r="G619" s="31">
         <f t="shared" si="33"/>
         <v>1.4101505699747101E-4</v>
       </c>
-      <c r="H619" s="42">
+      <c r="H619" s="31">
         <f t="shared" si="33"/>
         <v>1.7935342093196896E-4</v>
       </c>
-      <c r="I619" s="43">
+      <c r="I619" s="32">
         <f t="shared" si="33"/>
         <v>1.7316336117647388</v>
       </c>
-      <c r="J619" s="44">
+      <c r="J619" s="33">
         <f t="shared" si="33"/>
         <v>9.0116403500478896E-3</v>
       </c>
-      <c r="K619" s="44">
+      <c r="K619" s="33">
         <f t="shared" si="33"/>
         <v>8.2848166579325266E-3</v>
       </c>
@@ -24710,36 +24721,36 @@
       <c r="B620" s="9">
         <v>10</v>
       </c>
-      <c r="C620" s="38"/>
-      <c r="D620" s="40">
+      <c r="C620" s="45"/>
+      <c r="D620" s="29">
         <f t="shared" ref="D620:K620" si="34">D613/10</f>
         <v>6.1227971475464119E-2</v>
       </c>
-      <c r="E620" s="40">
+      <c r="E620" s="29">
         <f t="shared" si="34"/>
         <v>7.403275491294245E-2</v>
       </c>
-      <c r="F620" s="41">
+      <c r="F620" s="30">
         <f t="shared" si="34"/>
         <v>7.2804720840312419E-4</v>
       </c>
-      <c r="G620" s="42">
+      <c r="G620" s="31">
         <f t="shared" si="34"/>
         <v>6.3073476993107011E-5</v>
       </c>
-      <c r="H620" s="42">
+      <c r="H620" s="31">
         <f t="shared" si="34"/>
         <v>7.5341208272763967E-5</v>
       </c>
-      <c r="I620" s="43">
+      <c r="I620" s="32">
         <f t="shared" si="34"/>
         <v>1.3985795705348458</v>
       </c>
-      <c r="J620" s="44">
+      <c r="J620" s="33">
         <f t="shared" si="34"/>
         <v>5.1023309562881671E-3</v>
       </c>
-      <c r="K620" s="44">
+      <c r="K620" s="33">
         <f t="shared" si="34"/>
         <v>6.1693962427453262E-3</v>
       </c>
@@ -24751,36 +24762,36 @@
       <c r="B621" s="9">
         <v>6</v>
       </c>
-      <c r="C621" s="38"/>
-      <c r="D621" s="40">
+      <c r="C621" s="45"/>
+      <c r="D621" s="29">
         <f t="shared" ref="D621:K621" si="35">D614/10</f>
         <v>0.13270620586845225</v>
       </c>
-      <c r="E621" s="40">
+      <c r="E621" s="29">
         <f t="shared" si="35"/>
         <v>0.1631994870672098</v>
       </c>
-      <c r="F621" s="41">
+      <c r="F621" s="30">
         <f t="shared" si="35"/>
         <v>4.2375500880114866E-4</v>
       </c>
-      <c r="G621" s="42">
+      <c r="G621" s="31">
         <f t="shared" si="35"/>
         <v>4.2207083895952832E-5</v>
       </c>
-      <c r="H621" s="42">
+      <c r="H621" s="31">
         <f t="shared" si="35"/>
         <v>6.198640041170321E-5</v>
       </c>
-      <c r="I621" s="43">
+      <c r="I621" s="32">
         <f t="shared" si="35"/>
         <v>1.8929898461726526</v>
       </c>
-      <c r="J621" s="44">
+      <c r="J621" s="33">
         <f t="shared" si="35"/>
         <v>8.2941378667782655E-3</v>
       </c>
-      <c r="K621" s="44">
+      <c r="K621" s="33">
         <f t="shared" si="35"/>
         <v>1.0199967941700612E-2</v>
       </c>
@@ -24792,53 +24803,53 @@
       <c r="B622" s="9">
         <v>10</v>
       </c>
-      <c r="C622" s="38"/>
-      <c r="D622" s="40">
+      <c r="C622" s="45"/>
+      <c r="D622" s="29">
         <f t="shared" ref="D622:K622" si="36">D615/10</f>
         <v>8.3248367065068871E-2</v>
       </c>
-      <c r="E622" s="40">
+      <c r="E622" s="29">
         <f t="shared" si="36"/>
         <v>8.9260305040929841E-2</v>
       </c>
-      <c r="F622" s="41">
+      <c r="F622" s="30">
         <f t="shared" si="36"/>
         <v>3.4889624396273599E-4</v>
       </c>
-      <c r="G622" s="42">
+      <c r="G622" s="31">
         <f t="shared" si="36"/>
         <v>2.1433580755440747E-5</v>
       </c>
-      <c r="H622" s="42">
+      <c r="H622" s="31">
         <f t="shared" si="36"/>
         <v>2.5082012598673181E-5</v>
       </c>
-      <c r="I622" s="43">
+      <c r="I622" s="32">
         <f t="shared" si="36"/>
         <v>1.349224242085294</v>
       </c>
-      <c r="J622" s="44">
+      <c r="J622" s="33">
         <f t="shared" si="36"/>
         <v>5.2030229415668044E-3</v>
       </c>
-      <c r="K622" s="44">
+      <c r="K622" s="33">
         <f t="shared" si="36"/>
         <v>5.5787690650581151E-3</v>
       </c>
     </row>
     <row r="623" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="624" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C624" s="45" t="s">
+      <c r="C624" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="D624" s="45"/>
-      <c r="E624" s="45"/>
-      <c r="F624" s="45"/>
-      <c r="G624" s="45"/>
-      <c r="H624" s="45"/>
-      <c r="I624" s="45"/>
-      <c r="J624" s="45"/>
-      <c r="K624" s="45"/>
+      <c r="D624" s="46"/>
+      <c r="E624" s="46"/>
+      <c r="F624" s="46"/>
+      <c r="G624" s="46"/>
+      <c r="H624" s="46"/>
+      <c r="I624" s="46"/>
+      <c r="J624" s="46"/>
+      <c r="K624" s="46"/>
     </row>
     <row r="625" spans="1:11" ht="29" x14ac:dyDescent="0.45">
       <c r="A625" s="9">
@@ -24847,38 +24858,38 @@
       <c r="B625" s="9">
         <v>6</v>
       </c>
-      <c r="C625" s="46">
+      <c r="C625" s="47">
         <v>0.95</v>
       </c>
-      <c r="D625" s="47" t="str">
+      <c r="D625" s="34" t="str">
         <f>"["&amp;ROUND(D603-1.96*D617, 4)&amp;", "&amp;ROUND(D603+1.96*D617, 4)&amp;"]"</f>
         <v>[3.4187, 3.6514]</v>
       </c>
-      <c r="E625" s="47" t="str">
+      <c r="E625" s="34" t="str">
         <f t="shared" ref="E625:K625" si="37">"["&amp;ROUND(E603-1.96*E617, 4)&amp;", "&amp;ROUND(E603+1.96*E617, 4)&amp;"]"</f>
         <v>[3.3443, 3.6307]</v>
       </c>
-      <c r="F625" s="48" t="str">
+      <c r="F625" s="35" t="str">
         <f t="shared" si="37"/>
         <v>[0.9306, 0.9354]</v>
       </c>
-      <c r="G625" s="48" t="str">
+      <c r="G625" s="35" t="str">
         <f>"["&amp;ROUND(G603-1.96*G617, 6)&amp;", "&amp;ROUND(G603+1.96*G617, 6)&amp;"]"</f>
         <v>[0.009377, 0.011066]</v>
       </c>
-      <c r="H625" s="48" t="str">
+      <c r="H625" s="35" t="str">
         <f t="shared" ref="H625:H630" si="38">"["&amp;ROUND(H603-1.96*H617, 6)&amp;", "&amp;ROUND(H603+1.96*H617, 6)&amp;"]"</f>
         <v>[0.009473, 0.01221]</v>
       </c>
-      <c r="I625" s="49" t="str">
+      <c r="I625" s="36" t="str">
         <f t="shared" si="37"/>
         <v>[96.319, 103.4146]</v>
       </c>
-      <c r="J625" s="50" t="str">
+      <c r="J625" s="37" t="str">
         <f t="shared" si="37"/>
         <v>[0.4273, 0.4564]</v>
       </c>
-      <c r="K625" s="50" t="str">
+      <c r="K625" s="37" t="str">
         <f t="shared" si="37"/>
         <v>[0.418, 0.4538]</v>
       </c>
@@ -24890,36 +24901,36 @@
       <c r="B626" s="9">
         <v>10</v>
       </c>
-      <c r="C626" s="38"/>
-      <c r="D626" s="47" t="str">
+      <c r="C626" s="45"/>
+      <c r="D626" s="34" t="str">
         <f t="shared" ref="D626:K626" si="39">"["&amp;ROUND(D604-1.96*D618, 4)&amp;", "&amp;ROUND(D604+1.96*D618, 4)&amp;"]"</f>
         <v>[3.397, 3.58]</v>
       </c>
-      <c r="E626" s="47" t="str">
+      <c r="E626" s="34" t="str">
         <f t="shared" si="39"/>
         <v>[3.3422, 3.5148]</v>
       </c>
-      <c r="F626" s="48" t="str">
+      <c r="F626" s="35" t="str">
         <f t="shared" si="39"/>
         <v>[0.9179, 0.9223]</v>
       </c>
-      <c r="G626" s="48" t="str">
-        <f t="shared" ref="G626:H626" si="40">"["&amp;ROUND(G604-1.96*G618, 6)&amp;", "&amp;ROUND(G604+1.96*G618, 6)&amp;"]"</f>
+      <c r="G626" s="35" t="str">
+        <f t="shared" ref="G626" si="40">"["&amp;ROUND(G604-1.96*G618, 6)&amp;", "&amp;ROUND(G604+1.96*G618, 6)&amp;"]"</f>
         <v>[0.006456, 0.007313]</v>
       </c>
-      <c r="H626" s="48" t="str">
+      <c r="H626" s="35" t="str">
         <f t="shared" si="38"/>
         <v>[0.006449, 0.007253]</v>
       </c>
-      <c r="I626" s="49" t="str">
+      <c r="I626" s="36" t="str">
         <f t="shared" si="39"/>
         <v>[98.0874, 103.8454]</v>
       </c>
-      <c r="J626" s="50" t="str">
+      <c r="J626" s="37" t="str">
         <f t="shared" si="39"/>
         <v>[0.4246, 0.4475]</v>
       </c>
-      <c r="K626" s="50" t="str">
+      <c r="K626" s="37" t="str">
         <f t="shared" si="39"/>
         <v>[0.4178, 0.4393]</v>
       </c>
@@ -24931,36 +24942,36 @@
       <c r="B627" s="9">
         <v>6</v>
       </c>
-      <c r="C627" s="38"/>
-      <c r="D627" s="47" t="str">
+      <c r="C627" s="45"/>
+      <c r="D627" s="34" t="str">
         <f t="shared" ref="D627:K627" si="41">"["&amp;ROUND(D605-1.96*D619, 4)&amp;", "&amp;ROUND(D605+1.96*D619, 4)&amp;"]"</f>
         <v>[5.3586, 5.7825]</v>
       </c>
-      <c r="E627" s="47" t="str">
+      <c r="E627" s="34" t="str">
         <f t="shared" si="41"/>
         <v>[5.1221, 5.5118]</v>
       </c>
-      <c r="F627" s="48" t="str">
+      <c r="F627" s="35" t="str">
         <f t="shared" si="41"/>
         <v>[0.9552, 0.9579]</v>
       </c>
-      <c r="G627" s="48" t="str">
-        <f t="shared" ref="G627:H627" si="42">"["&amp;ROUND(G605-1.96*G619, 6)&amp;", "&amp;ROUND(G605+1.96*G619, 6)&amp;"]"</f>
+      <c r="G627" s="35" t="str">
+        <f t="shared" ref="G627" si="42">"["&amp;ROUND(G605-1.96*G619, 6)&amp;", "&amp;ROUND(G605+1.96*G619, 6)&amp;"]"</f>
         <v>[0.002289, 0.002841]</v>
       </c>
-      <c r="H627" s="48" t="str">
+      <c r="H627" s="35" t="str">
         <f t="shared" si="38"/>
         <v>[0.002599, 0.003302]</v>
       </c>
-      <c r="I627" s="49" t="str">
+      <c r="I627" s="36" t="str">
         <f t="shared" si="41"/>
         <v>[87.5863, 94.3743]</v>
       </c>
-      <c r="J627" s="50" t="str">
+      <c r="J627" s="37" t="str">
         <f t="shared" si="41"/>
         <v>[0.4465, 0.4819]</v>
       </c>
-      <c r="K627" s="50" t="str">
+      <c r="K627" s="37" t="str">
         <f t="shared" si="41"/>
         <v>[0.4268, 0.4593]</v>
       </c>
@@ -24972,36 +24983,36 @@
       <c r="B628" s="9">
         <v>10</v>
       </c>
-      <c r="C628" s="38"/>
-      <c r="D628" s="47" t="str">
+      <c r="C628" s="45"/>
+      <c r="D628" s="34" t="str">
         <f t="shared" ref="D628:K628" si="43">"["&amp;ROUND(D606-1.96*D620, 4)&amp;", "&amp;ROUND(D606+1.96*D620, 4)&amp;"]"</f>
         <v>[5.443, 5.683]</v>
       </c>
-      <c r="E628" s="47" t="str">
+      <c r="E628" s="34" t="str">
         <f t="shared" si="43"/>
         <v>[5.4283, 5.7185]</v>
       </c>
-      <c r="F628" s="48" t="str">
+      <c r="F628" s="35" t="str">
         <f t="shared" si="43"/>
         <v>[0.9489, 0.9518]</v>
       </c>
-      <c r="G628" s="48" t="str">
-        <f t="shared" ref="G628:H628" si="44">"["&amp;ROUND(G606-1.96*G620, 6)&amp;", "&amp;ROUND(G606+1.96*G620, 6)&amp;"]"</f>
+      <c r="G628" s="35" t="str">
+        <f t="shared" ref="G628" si="44">"["&amp;ROUND(G606-1.96*G620, 6)&amp;", "&amp;ROUND(G606+1.96*G620, 6)&amp;"]"</f>
         <v>[0.001525, 0.001772]</v>
       </c>
-      <c r="H628" s="48" t="str">
+      <c r="H628" s="35" t="str">
         <f t="shared" si="38"/>
         <v>[0.001642, 0.001937]</v>
       </c>
-      <c r="I628" s="49" t="str">
+      <c r="I628" s="36" t="str">
         <f t="shared" si="43"/>
         <v>[91.2268, 96.7092]</v>
       </c>
-      <c r="J628" s="50" t="str">
+      <c r="J628" s="37" t="str">
         <f t="shared" si="43"/>
         <v>[0.4536, 0.4736]</v>
       </c>
-      <c r="K628" s="50" t="str">
+      <c r="K628" s="37" t="str">
         <f t="shared" si="43"/>
         <v>[0.4524, 0.4765]</v>
       </c>
@@ -25013,36 +25024,36 @@
       <c r="B629" s="9">
         <v>6</v>
       </c>
-      <c r="C629" s="38"/>
-      <c r="D629" s="47" t="str">
+      <c r="C629" s="45"/>
+      <c r="D629" s="34" t="str">
         <f t="shared" ref="D629:K629" si="45">"["&amp;ROUND(D607-1.96*D621, 4)&amp;", "&amp;ROUND(D607+1.96*D621, 4)&amp;"]"</f>
         <v>[7.1827, 7.7029]</v>
       </c>
-      <c r="E629" s="47" t="str">
+      <c r="E629" s="34" t="str">
         <f t="shared" si="45"/>
         <v>[7.124, 7.7638]</v>
       </c>
-      <c r="F629" s="48" t="str">
+      <c r="F629" s="35" t="str">
         <f t="shared" si="45"/>
         <v>[0.9677, 0.9694]</v>
       </c>
-      <c r="G629" s="48" t="str">
-        <f t="shared" ref="G629:H629" si="46">"["&amp;ROUND(G607-1.96*G621, 6)&amp;", "&amp;ROUND(G607+1.96*G621, 6)&amp;"]"</f>
+      <c r="G629" s="35" t="str">
+        <f t="shared" ref="G629" si="46">"["&amp;ROUND(G607-1.96*G621, 6)&amp;", "&amp;ROUND(G607+1.96*G621, 6)&amp;"]"</f>
         <v>[0.000707, 0.000872]</v>
       </c>
-      <c r="H629" s="48" t="str">
+      <c r="H629" s="35" t="str">
         <f t="shared" si="38"/>
         <v>[0.000872, 0.001115]</v>
       </c>
-      <c r="I629" s="49" t="str">
+      <c r="I629" s="36" t="str">
         <f t="shared" si="45"/>
         <v>[81.6997, 89.1202]</v>
       </c>
-      <c r="J629" s="50" t="str">
+      <c r="J629" s="37" t="str">
         <f t="shared" si="45"/>
         <v>[0.4489, 0.4814]</v>
       </c>
-      <c r="K629" s="50" t="str">
+      <c r="K629" s="37" t="str">
         <f t="shared" si="45"/>
         <v>[0.4453, 0.4852]</v>
       </c>
@@ -25054,42 +25065,43 @@
       <c r="B630" s="9">
         <v>10</v>
       </c>
-      <c r="C630" s="38"/>
-      <c r="D630" s="47" t="str">
+      <c r="C630" s="45"/>
+      <c r="D630" s="34" t="str">
         <f t="shared" ref="D630:K630" si="47">"["&amp;ROUND(D608-1.96*D622, 4)&amp;", "&amp;ROUND(D608+1.96*D622, 4)&amp;"]"</f>
         <v>[7.3214, 7.6478]</v>
       </c>
-      <c r="E630" s="47" t="str">
+      <c r="E630" s="34" t="str">
         <f t="shared" si="47"/>
         <v>[7.3392, 7.6891]</v>
       </c>
-      <c r="F630" s="48" t="str">
+      <c r="F630" s="35" t="str">
         <f t="shared" si="47"/>
         <v>[0.962, 0.9634]</v>
       </c>
-      <c r="G630" s="48" t="str">
-        <f t="shared" ref="G630:H630" si="48">"["&amp;ROUND(G608-1.96*G622, 6)&amp;", "&amp;ROUND(G608+1.96*G622, 6)&amp;"]"</f>
+      <c r="G630" s="35" t="str">
+        <f t="shared" ref="G630" si="48">"["&amp;ROUND(G608-1.96*G622, 6)&amp;", "&amp;ROUND(G608+1.96*G622, 6)&amp;"]"</f>
         <v>[0.000488, 0.000572]</v>
       </c>
-      <c r="H630" s="48" t="str">
+      <c r="H630" s="35" t="str">
         <f t="shared" si="38"/>
         <v>[0.000536, 0.000635]</v>
       </c>
-      <c r="I630" s="49" t="str">
+      <c r="I630" s="36" t="str">
         <f t="shared" si="47"/>
         <v>[89.5028, 94.7917]</v>
       </c>
-      <c r="J630" s="50" t="str">
+      <c r="J630" s="37" t="str">
         <f t="shared" si="47"/>
         <v>[0.4576, 0.478]</v>
       </c>
-      <c r="K630" s="50" t="str">
+      <c r="K630" s="37" t="str">
         <f t="shared" si="47"/>
         <v>[0.4587, 0.4806]</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="M101:Q116"/>
     <mergeCell ref="M47:Q62"/>
     <mergeCell ref="C617:C622"/>
     <mergeCell ref="C624:K624"/>
@@ -25106,7 +25118,6 @@
     <mergeCell ref="M82:Q82"/>
     <mergeCell ref="M83:Q98"/>
     <mergeCell ref="M100:Q100"/>
-    <mergeCell ref="M101:Q116"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>